<commit_message>
Added: pur_inv & sale_inv builders
</commit_message>
<xml_diff>
--- a/invoice-python/Update.xlsx
+++ b/invoice-python/Update.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="151">
   <si>
     <t>INVOICE</t>
   </si>
@@ -101,37 +101,76 @@
     <t>4x40'</t>
   </si>
   <si>
+    <t>BILL</t>
+  </si>
+  <si>
     <t>PARTY NAME</t>
   </si>
   <si>
+    <t>GRADE</t>
+  </si>
+  <si>
     <t>SIZE</t>
   </si>
   <si>
-    <t>PIECES</t>
-  </si>
-  <si>
-    <t>p1</t>
-  </si>
-  <si>
-    <t>p2</t>
-  </si>
-  <si>
-    <t>p3</t>
-  </si>
-  <si>
-    <t>p4</t>
-  </si>
-  <si>
-    <t>p5</t>
-  </si>
-  <si>
-    <t>p6</t>
-  </si>
-  <si>
-    <t>p7</t>
-  </si>
-  <si>
-    <t>p8</t>
+    <t>PCS</t>
+  </si>
+  <si>
+    <t>Bill-1</t>
+  </si>
+  <si>
+    <t>Bill-2</t>
+  </si>
+  <si>
+    <t>Bill-3</t>
+  </si>
+  <si>
+    <t>Bill-4</t>
+  </si>
+  <si>
+    <t>Bill-5</t>
+  </si>
+  <si>
+    <t>Bill-6</t>
+  </si>
+  <si>
+    <t>Bill-7</t>
+  </si>
+  <si>
+    <t>Bill-8</t>
+  </si>
+  <si>
+    <t>Party-1</t>
+  </si>
+  <si>
+    <t>Party-2</t>
+  </si>
+  <si>
+    <t>Party-3</t>
+  </si>
+  <si>
+    <t>Party-4</t>
+  </si>
+  <si>
+    <t>Party-5</t>
+  </si>
+  <si>
+    <t>Party-6</t>
+  </si>
+  <si>
+    <t>Party-7</t>
+  </si>
+  <si>
+    <t>Party-8</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
   </si>
   <si>
     <t>f-001(200)</t>
@@ -1396,13 +1435,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E138"/>
+  <dimension ref="A1:G138"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="B1" s="1" t="s">
         <v>28</v>
       </c>
@@ -1413,2336 +1452,3164 @@
         <v>30</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>31</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>200</v>
       </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="G2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>800</v>
       </c>
-      <c r="E3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="G3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>51</v>
+      </c>
+      <c r="E4" t="s">
         <v>11</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>200</v>
       </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="G4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>250</v>
       </c>
-      <c r="E5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="G5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>200</v>
       </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="G6" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" t="s">
         <v>8</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>500</v>
       </c>
-      <c r="E7" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="G7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
         <v>2</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>1000</v>
       </c>
-      <c r="E8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="G8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" t="s">
         <v>5</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>2000</v>
       </c>
-      <c r="E9" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s">
         <v>7</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>2000</v>
       </c>
-      <c r="E10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="G10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" t="s">
         <v>8</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>6700</v>
       </c>
-      <c r="E11" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="G11" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" t="s">
         <v>9</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>400</v>
       </c>
-      <c r="E12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="G12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" t="s">
         <v>3</v>
       </c>
-      <c r="D13">
+      <c r="F13">
         <v>750</v>
       </c>
-      <c r="E13" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="G13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
         <v>5</v>
       </c>
-      <c r="D14">
+      <c r="F14">
         <v>2000</v>
       </c>
-      <c r="E14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="G14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" t="s">
         <v>7</v>
       </c>
-      <c r="D15">
+      <c r="F15">
         <v>3000</v>
       </c>
-      <c r="E15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="G15" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>50</v>
+      </c>
+      <c r="E16" t="s">
         <v>8</v>
       </c>
-      <c r="D16">
+      <c r="F16">
         <v>2000</v>
       </c>
-      <c r="E16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="G16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>51</v>
+      </c>
+      <c r="E17" t="s">
         <v>2</v>
       </c>
-      <c r="D17">
+      <c r="F17">
         <v>1000</v>
       </c>
-      <c r="E17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="G17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" t="s">
         <v>5</v>
       </c>
-      <c r="D18">
+      <c r="F18">
         <v>500</v>
       </c>
-      <c r="E18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="G18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" t="s">
         <v>7</v>
       </c>
-      <c r="D19">
+      <c r="F19">
         <v>400</v>
       </c>
-      <c r="E19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="G19" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C20" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" t="s">
         <v>8</v>
       </c>
-      <c r="D20">
+      <c r="F20">
         <v>300</v>
       </c>
-      <c r="E20" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="G20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C21" t="s">
+        <v>46</v>
+      </c>
+      <c r="D21" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" t="s">
         <v>11</v>
       </c>
-      <c r="D21">
+      <c r="F21">
         <v>500</v>
       </c>
-      <c r="E21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="G21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" t="s">
         <v>11</v>
       </c>
-      <c r="D22">
+      <c r="F22">
         <v>500</v>
       </c>
-      <c r="E22" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="G22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E23" t="s">
         <v>2</v>
       </c>
-      <c r="D23">
+      <c r="F23">
         <v>8000</v>
       </c>
-      <c r="E23" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="G23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" t="s">
         <v>4</v>
       </c>
-      <c r="D24">
+      <c r="F24">
         <v>1500</v>
       </c>
-      <c r="E24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="G24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C25" t="s">
+        <v>47</v>
+      </c>
+      <c r="D25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" t="s">
         <v>8</v>
       </c>
-      <c r="D25">
+      <c r="F25">
         <v>500</v>
       </c>
-      <c r="E25" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="G25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" t="s">
+        <v>50</v>
+      </c>
+      <c r="E26" t="s">
         <v>5</v>
       </c>
-      <c r="D26">
+      <c r="F26">
         <v>1000</v>
       </c>
-      <c r="E26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="G26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C27" t="s">
+        <v>47</v>
+      </c>
+      <c r="D27" t="s">
+        <v>51</v>
+      </c>
+      <c r="E27" t="s">
         <v>7</v>
       </c>
-      <c r="D27">
+      <c r="F27">
         <v>1000</v>
       </c>
-      <c r="E27" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="G27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C28" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" t="s">
         <v>8</v>
       </c>
-      <c r="D28">
+      <c r="F28">
         <v>1000</v>
       </c>
-      <c r="E28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="G28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
+        <v>47</v>
+      </c>
+      <c r="D29" t="s">
+        <v>50</v>
+      </c>
+      <c r="E29" t="s">
         <v>11</v>
       </c>
-      <c r="D29">
+      <c r="F29">
         <v>1400</v>
       </c>
-      <c r="E29" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="G29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C30" t="s">
+        <v>47</v>
+      </c>
+      <c r="D30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" t="s">
         <v>12</v>
       </c>
-      <c r="D30">
-        <v>50</v>
-      </c>
-      <c r="E30" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30">
+        <v>50</v>
+      </c>
+      <c r="G30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" t="s">
         <v>2</v>
       </c>
-      <c r="D31">
+      <c r="F31">
         <v>3000</v>
       </c>
-      <c r="E31" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="G31" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C32" t="s">
+        <v>47</v>
+      </c>
+      <c r="D32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" t="s">
         <v>5</v>
       </c>
-      <c r="D32">
+      <c r="F32">
         <v>150</v>
       </c>
-      <c r="E32" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="G32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" t="s">
+        <v>50</v>
+      </c>
+      <c r="E33" t="s">
         <v>3</v>
       </c>
-      <c r="D33">
+      <c r="F33">
         <v>100</v>
       </c>
-      <c r="E33" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="G33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C34" t="s">
+        <v>47</v>
+      </c>
+      <c r="D34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" t="s">
         <v>2</v>
       </c>
-      <c r="D34">
+      <c r="F34">
         <v>3000</v>
       </c>
-      <c r="E34" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="G34" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" t="s">
         <v>5</v>
       </c>
-      <c r="D35">
+      <c r="F35">
         <v>600</v>
       </c>
-      <c r="E35" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="G35" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C36" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" t="s">
+        <v>50</v>
+      </c>
+      <c r="E36" t="s">
         <v>2</v>
       </c>
-      <c r="D36">
+      <c r="F36">
         <v>13000</v>
       </c>
-      <c r="E36" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="G36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
+        <v>47</v>
+      </c>
+      <c r="D37" t="s">
+        <v>51</v>
+      </c>
+      <c r="E37" t="s">
         <v>4</v>
       </c>
-      <c r="D37">
+      <c r="F37">
         <v>3000</v>
       </c>
-      <c r="E37" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="G37" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C38" t="s">
+        <v>47</v>
+      </c>
+      <c r="D38" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" t="s">
         <v>5</v>
       </c>
-      <c r="D38">
+      <c r="F38">
         <v>1000</v>
       </c>
-      <c r="E38" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="G38" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C39" t="s">
+        <v>47</v>
+      </c>
+      <c r="D39" t="s">
+        <v>50</v>
+      </c>
+      <c r="E39" t="s">
         <v>7</v>
       </c>
-      <c r="D39">
+      <c r="F39">
         <v>500</v>
       </c>
-      <c r="E39" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="G39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s">
+        <v>47</v>
+      </c>
+      <c r="D40" t="s">
+        <v>50</v>
+      </c>
+      <c r="E40" t="s">
         <v>8</v>
       </c>
-      <c r="D40">
+      <c r="F40">
         <v>250</v>
       </c>
-      <c r="E40" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
+      <c r="G40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" t="s">
+        <v>51</v>
+      </c>
+      <c r="E41" t="s">
         <v>2</v>
       </c>
-      <c r="D41">
+      <c r="F41">
         <v>1000</v>
       </c>
-      <c r="E41" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="G41" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C42" t="s">
+        <v>47</v>
+      </c>
+      <c r="D42" t="s">
+        <v>49</v>
+      </c>
+      <c r="E42" t="s">
         <v>4</v>
       </c>
-      <c r="D42">
+      <c r="F42">
         <v>500</v>
       </c>
-      <c r="E42" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
+      <c r="G42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C43" t="s">
+        <v>47</v>
+      </c>
+      <c r="D43" t="s">
+        <v>50</v>
+      </c>
+      <c r="E43" t="s">
         <v>5</v>
       </c>
-      <c r="D43">
+      <c r="F43">
         <v>100</v>
       </c>
-      <c r="E43" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
+      <c r="G43" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
+        <v>47</v>
+      </c>
+      <c r="D44" t="s">
+        <v>51</v>
+      </c>
+      <c r="E44" t="s">
         <v>7</v>
       </c>
-      <c r="D44">
+      <c r="F44">
         <v>100</v>
       </c>
-      <c r="E44" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
+      <c r="G44" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C45" t="s">
+        <v>47</v>
+      </c>
+      <c r="D45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E45" t="s">
         <v>8</v>
       </c>
-      <c r="D45">
-        <v>50</v>
-      </c>
-      <c r="E45" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+      <c r="F45">
+        <v>50</v>
+      </c>
+      <c r="G45" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C46" t="s">
+        <v>47</v>
+      </c>
+      <c r="D46" t="s">
+        <v>50</v>
+      </c>
+      <c r="E46" t="s">
         <v>5</v>
       </c>
-      <c r="D46">
+      <c r="F46">
         <v>2450</v>
       </c>
-      <c r="E46" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
+      <c r="G46" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D47" t="s">
+        <v>51</v>
+      </c>
+      <c r="E47" t="s">
         <v>2</v>
       </c>
-      <c r="D47">
+      <c r="F47">
         <v>5000</v>
       </c>
-      <c r="E47" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
+      <c r="G47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C48" t="s">
+        <v>47</v>
+      </c>
+      <c r="D48" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" t="s">
         <v>4</v>
       </c>
-      <c r="D48">
+      <c r="F48">
         <v>3000</v>
       </c>
-      <c r="E48" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
+      <c r="G48" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C49" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49" t="s">
+        <v>50</v>
+      </c>
+      <c r="E49" t="s">
         <v>5</v>
       </c>
-      <c r="D49">
+      <c r="F49">
         <v>2000</v>
       </c>
-      <c r="E49" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+      <c r="G49" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C50" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50" t="s">
+        <v>50</v>
+      </c>
+      <c r="E50" t="s">
         <v>7</v>
       </c>
-      <c r="D50">
+      <c r="F50">
         <v>350</v>
       </c>
-      <c r="E50" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
+      <c r="G50" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C51" t="s">
+        <v>47</v>
+      </c>
+      <c r="D51" t="s">
+        <v>51</v>
+      </c>
+      <c r="E51" t="s">
         <v>8</v>
       </c>
-      <c r="D51">
+      <c r="F51">
         <v>400</v>
       </c>
-      <c r="E51" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
+      <c r="G51" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C52" t="s">
+        <v>47</v>
+      </c>
+      <c r="D52" t="s">
+        <v>50</v>
+      </c>
+      <c r="E52" t="s">
         <v>5</v>
       </c>
-      <c r="D52">
+      <c r="F52">
         <v>300</v>
       </c>
-      <c r="E52" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+      <c r="G52" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C53" t="s">
+        <v>47</v>
+      </c>
+      <c r="D53" t="s">
+        <v>50</v>
+      </c>
+      <c r="E53" t="s">
         <v>7</v>
       </c>
-      <c r="D53">
+      <c r="F53">
         <v>400</v>
       </c>
-      <c r="E53" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
+      <c r="G53" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C54" t="s">
+        <v>47</v>
+      </c>
+      <c r="D54" t="s">
+        <v>49</v>
+      </c>
+      <c r="E54" t="s">
         <v>8</v>
       </c>
-      <c r="D54">
+      <c r="F54">
         <v>200</v>
       </c>
-      <c r="E54" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
+      <c r="G54" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C55" t="s">
+        <v>47</v>
+      </c>
+      <c r="D55" t="s">
+        <v>50</v>
+      </c>
+      <c r="E55" t="s">
         <v>7</v>
       </c>
-      <c r="D55">
+      <c r="F55">
         <v>10250</v>
       </c>
-      <c r="E55" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
+      <c r="G55" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C56" t="s">
+        <v>47</v>
+      </c>
+      <c r="D56" t="s">
+        <v>50</v>
+      </c>
+      <c r="E56" t="s">
         <v>8</v>
       </c>
-      <c r="D56">
+      <c r="F56">
         <v>4000</v>
       </c>
-      <c r="E56" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+      <c r="G56" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C57" t="s">
+        <v>47</v>
+      </c>
+      <c r="D57" t="s">
+        <v>51</v>
+      </c>
+      <c r="E57" t="s">
         <v>9</v>
       </c>
-      <c r="D57">
+      <c r="F57">
         <v>800</v>
       </c>
-      <c r="E57" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+      <c r="G57" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C58" t="s">
+        <v>47</v>
+      </c>
+      <c r="D58" t="s">
+        <v>49</v>
+      </c>
+      <c r="E58" t="s">
         <v>2</v>
       </c>
-      <c r="D58">
+      <c r="F58">
         <v>1050</v>
       </c>
-      <c r="E58" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
+      <c r="G58" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D59" t="s">
+        <v>50</v>
+      </c>
+      <c r="E59" t="s">
         <v>4</v>
       </c>
-      <c r="D59">
+      <c r="F59">
         <v>700</v>
       </c>
-      <c r="E59" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
+      <c r="G59" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="1">
         <v>58</v>
       </c>
       <c r="B60" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C60" t="s">
+        <v>47</v>
+      </c>
+      <c r="D60" t="s">
+        <v>50</v>
+      </c>
+      <c r="E60" t="s">
         <v>8</v>
       </c>
-      <c r="D60">
+      <c r="F60">
         <v>650</v>
       </c>
-      <c r="E60" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
+      <c r="G60" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" s="1">
         <v>59</v>
       </c>
       <c r="B61" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C61" t="s">
+        <v>47</v>
+      </c>
+      <c r="D61" t="s">
+        <v>51</v>
+      </c>
+      <c r="E61" t="s">
         <v>2</v>
       </c>
-      <c r="D61">
+      <c r="F61">
         <v>150</v>
       </c>
-      <c r="E61" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+      <c r="G61" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C62" t="s">
+        <v>47</v>
+      </c>
+      <c r="D62" t="s">
+        <v>49</v>
+      </c>
+      <c r="E62" t="s">
         <v>4</v>
       </c>
-      <c r="D62">
+      <c r="F62">
         <v>3050</v>
       </c>
-      <c r="E62" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
+      <c r="G62" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C63" t="s">
+        <v>47</v>
+      </c>
+      <c r="D63" t="s">
+        <v>50</v>
+      </c>
+      <c r="E63" t="s">
         <v>7</v>
       </c>
-      <c r="D63">
+      <c r="F63">
         <v>100</v>
       </c>
-      <c r="E63" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
+      <c r="G63" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C64" t="s">
+        <v>47</v>
+      </c>
+      <c r="D64" t="s">
+        <v>51</v>
+      </c>
+      <c r="E64" t="s">
         <v>5</v>
       </c>
-      <c r="D64">
+      <c r="F64">
         <v>200</v>
       </c>
-      <c r="E64" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="G64" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C65" t="s">
+        <v>47</v>
+      </c>
+      <c r="D65" t="s">
+        <v>49</v>
+      </c>
+      <c r="E65" t="s">
         <v>7</v>
       </c>
-      <c r="D65">
+      <c r="F65">
         <v>300</v>
       </c>
-      <c r="E65" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+      <c r="G65" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C66" t="s">
+        <v>47</v>
+      </c>
+      <c r="D66" t="s">
+        <v>50</v>
+      </c>
+      <c r="E66" t="s">
         <v>8</v>
       </c>
-      <c r="D66">
+      <c r="F66">
         <v>300</v>
       </c>
-      <c r="E66" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5">
+      <c r="G66" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C67" t="s">
+        <v>47</v>
+      </c>
+      <c r="D67" t="s">
+        <v>51</v>
+      </c>
+      <c r="E67" t="s">
         <v>2</v>
       </c>
-      <c r="D67">
+      <c r="F67">
         <v>250</v>
       </c>
-      <c r="E67" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5">
+      <c r="G67" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C68" t="s">
+        <v>47</v>
+      </c>
+      <c r="D68" t="s">
+        <v>49</v>
+      </c>
+      <c r="E68" t="s">
         <v>2</v>
       </c>
-      <c r="D68">
+      <c r="F68">
         <v>1100</v>
       </c>
-      <c r="E68" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
+      <c r="G68" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" s="1">
         <v>67</v>
       </c>
       <c r="B69" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C69" t="s">
+        <v>47</v>
+      </c>
+      <c r="D69" t="s">
+        <v>50</v>
+      </c>
+      <c r="E69" t="s">
         <v>4</v>
       </c>
-      <c r="D69">
+      <c r="F69">
         <v>400</v>
       </c>
-      <c r="E69" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5">
+      <c r="G69" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C70" t="s">
+        <v>47</v>
+      </c>
+      <c r="D70" t="s">
+        <v>50</v>
+      </c>
+      <c r="E70" t="s">
         <v>4</v>
       </c>
-      <c r="D70">
+      <c r="F70">
         <v>100</v>
       </c>
-      <c r="E70" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5">
+      <c r="G70" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" s="1">
         <v>69</v>
       </c>
       <c r="B71" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C71" t="s">
+        <v>47</v>
+      </c>
+      <c r="D71" t="s">
+        <v>51</v>
+      </c>
+      <c r="E71" t="s">
         <v>2</v>
       </c>
-      <c r="D71">
+      <c r="F71">
         <v>3000</v>
       </c>
-      <c r="E71" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
+      <c r="G71" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" s="1">
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C72" t="s">
+        <v>47</v>
+      </c>
+      <c r="D72" t="s">
+        <v>50</v>
+      </c>
+      <c r="E72" t="s">
         <v>4</v>
       </c>
-      <c r="D72">
+      <c r="F72">
         <v>2500</v>
       </c>
-      <c r="E72" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5">
+      <c r="G72" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" s="1">
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C73" t="s">
+        <v>47</v>
+      </c>
+      <c r="D73" t="s">
+        <v>50</v>
+      </c>
+      <c r="E73" t="s">
         <v>5</v>
       </c>
-      <c r="D73">
+      <c r="F73">
         <v>1000</v>
       </c>
-      <c r="E73" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
+      <c r="G73" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C74" t="s">
+        <v>47</v>
+      </c>
+      <c r="D74" t="s">
+        <v>49</v>
+      </c>
+      <c r="E74" t="s">
         <v>7</v>
       </c>
-      <c r="D74">
+      <c r="F74">
         <v>1000</v>
       </c>
-      <c r="E74" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="G74" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" s="1">
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C75" t="s">
+        <v>47</v>
+      </c>
+      <c r="D75" t="s">
+        <v>50</v>
+      </c>
+      <c r="E75" t="s">
         <v>8</v>
       </c>
-      <c r="D75">
+      <c r="F75">
         <v>1000</v>
       </c>
-      <c r="E75" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
+      <c r="G75" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" s="1">
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C76" t="s">
+        <v>47</v>
+      </c>
+      <c r="D76" t="s">
+        <v>50</v>
+      </c>
+      <c r="E76" t="s">
         <v>11</v>
       </c>
-      <c r="D76">
+      <c r="F76">
         <v>500</v>
       </c>
-      <c r="E76" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5">
+      <c r="G76" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C77" t="s">
+        <v>47</v>
+      </c>
+      <c r="D77" t="s">
+        <v>51</v>
+      </c>
+      <c r="E77" t="s">
         <v>12</v>
       </c>
-      <c r="D77">
-        <v>50</v>
-      </c>
-      <c r="E77" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
+      <c r="F77">
+        <v>50</v>
+      </c>
+      <c r="G77" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C78" t="s">
+        <v>47</v>
+      </c>
+      <c r="D78" t="s">
+        <v>49</v>
+      </c>
+      <c r="E78" t="s">
         <v>7</v>
       </c>
-      <c r="D78">
+      <c r="F78">
         <v>600</v>
       </c>
-      <c r="E78" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
+      <c r="G78" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C79" t="s">
+        <v>47</v>
+      </c>
+      <c r="D79" t="s">
+        <v>50</v>
+      </c>
+      <c r="E79" t="s">
         <v>2</v>
       </c>
-      <c r="D79">
+      <c r="F79">
         <v>7000</v>
       </c>
-      <c r="E79" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
+      <c r="G79" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" s="1">
         <v>78</v>
       </c>
       <c r="B80" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C80" t="s">
+        <v>47</v>
+      </c>
+      <c r="D80" t="s">
+        <v>50</v>
+      </c>
+      <c r="E80" t="s">
         <v>4</v>
       </c>
-      <c r="D80">
+      <c r="F80">
         <v>2500</v>
       </c>
-      <c r="E80" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5">
+      <c r="G80" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C81" t="s">
+        <v>47</v>
+      </c>
+      <c r="D81" t="s">
+        <v>51</v>
+      </c>
+      <c r="E81" t="s">
         <v>5</v>
       </c>
-      <c r="D81">
+      <c r="F81">
         <v>1000</v>
       </c>
-      <c r="E81" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
+      <c r="G81" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C82" t="s">
+        <v>47</v>
+      </c>
+      <c r="D82" t="s">
+        <v>49</v>
+      </c>
+      <c r="E82" t="s">
         <v>6</v>
       </c>
-      <c r="D82">
+      <c r="F82">
         <v>500</v>
       </c>
-      <c r="E82" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5">
+      <c r="G82" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" s="1">
         <v>81</v>
       </c>
       <c r="B83" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C83" t="s">
+        <v>47</v>
+      </c>
+      <c r="D83" t="s">
+        <v>50</v>
+      </c>
+      <c r="E83" t="s">
         <v>7</v>
       </c>
-      <c r="D83">
+      <c r="F83">
         <v>2500</v>
       </c>
-      <c r="E83" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5">
+      <c r="G83" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" s="1">
         <v>82</v>
       </c>
       <c r="B84" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C84" t="s">
+        <v>47</v>
+      </c>
+      <c r="D84" t="s">
+        <v>51</v>
+      </c>
+      <c r="E84" t="s">
         <v>8</v>
       </c>
-      <c r="D84">
+      <c r="F84">
         <v>1200</v>
       </c>
-      <c r="E84" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="85" spans="1:5">
+      <c r="G84" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" s="1">
         <v>83</v>
       </c>
       <c r="B85" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C85" t="s">
+        <v>47</v>
+      </c>
+      <c r="D85" t="s">
+        <v>49</v>
+      </c>
+      <c r="E85" t="s">
         <v>4</v>
       </c>
-      <c r="D85">
+      <c r="F85">
         <v>500</v>
       </c>
-      <c r="E85" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5">
+      <c r="G85" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" s="1">
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C86" t="s">
+        <v>47</v>
+      </c>
+      <c r="D86" t="s">
+        <v>50</v>
+      </c>
+      <c r="E86" t="s">
         <v>2</v>
       </c>
-      <c r="D86">
+      <c r="F86">
         <v>500</v>
       </c>
-      <c r="E86" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
+      <c r="G86" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C87" t="s">
+        <v>47</v>
+      </c>
+      <c r="D87" t="s">
+        <v>51</v>
+      </c>
+      <c r="E87" t="s">
         <v>4</v>
       </c>
-      <c r="D87">
+      <c r="F87">
         <v>500</v>
       </c>
-      <c r="E87" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5">
+      <c r="G87" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C88" t="s">
+        <v>47</v>
+      </c>
+      <c r="D88" t="s">
+        <v>49</v>
+      </c>
+      <c r="E88" t="s">
         <v>7</v>
       </c>
-      <c r="D88">
+      <c r="F88">
         <v>150</v>
       </c>
-      <c r="E88" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5">
+      <c r="G88" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C89" t="s">
+        <v>47</v>
+      </c>
+      <c r="D89" t="s">
+        <v>50</v>
+      </c>
+      <c r="E89" t="s">
         <v>8</v>
       </c>
-      <c r="D89">
+      <c r="F89">
         <v>100</v>
       </c>
-      <c r="E89" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
+      <c r="G89" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C90" t="s">
+        <v>47</v>
+      </c>
+      <c r="D90" t="s">
+        <v>50</v>
+      </c>
+      <c r="E90" t="s">
         <v>2</v>
       </c>
-      <c r="D90">
+      <c r="F90">
         <v>1000</v>
       </c>
-      <c r="E90" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5">
+      <c r="G90" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" s="1">
         <v>89</v>
       </c>
       <c r="B91" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C91" t="s">
+        <v>47</v>
+      </c>
+      <c r="D91" t="s">
+        <v>51</v>
+      </c>
+      <c r="E91" t="s">
         <v>4</v>
       </c>
-      <c r="D91">
+      <c r="F91">
         <v>500</v>
       </c>
-      <c r="E91" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="92" spans="1:5">
+      <c r="G91" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C92" t="s">
+        <v>47</v>
+      </c>
+      <c r="D92" t="s">
+        <v>50</v>
+      </c>
+      <c r="E92" t="s">
         <v>2</v>
       </c>
-      <c r="D92">
+      <c r="F92">
         <v>2000</v>
       </c>
-      <c r="E92" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5">
+      <c r="G92" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C93" t="s">
+        <v>47</v>
+      </c>
+      <c r="D93" t="s">
+        <v>50</v>
+      </c>
+      <c r="E93" t="s">
         <v>4</v>
       </c>
-      <c r="D93">
+      <c r="F93">
         <v>1000</v>
       </c>
-      <c r="E93" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5">
+      <c r="G93" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C94" t="s">
+        <v>47</v>
+      </c>
+      <c r="D94" t="s">
+        <v>49</v>
+      </c>
+      <c r="E94" t="s">
         <v>7</v>
       </c>
-      <c r="D94">
+      <c r="F94">
         <v>250</v>
       </c>
-      <c r="E94" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="95" spans="1:5">
+      <c r="G94" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C95" t="s">
+        <v>47</v>
+      </c>
+      <c r="D95" t="s">
+        <v>50</v>
+      </c>
+      <c r="E95" t="s">
         <v>8</v>
       </c>
-      <c r="D95">
+      <c r="F95">
         <v>200</v>
       </c>
-      <c r="E95" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="96" spans="1:5">
+      <c r="G95" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C96" t="s">
+        <v>47</v>
+      </c>
+      <c r="D96" t="s">
+        <v>50</v>
+      </c>
+      <c r="E96" t="s">
         <v>7</v>
       </c>
-      <c r="D96">
+      <c r="F96">
         <v>1500</v>
       </c>
-      <c r="E96" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5">
+      <c r="G96" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C97" t="s">
+        <v>47</v>
+      </c>
+      <c r="D97" t="s">
+        <v>51</v>
+      </c>
+      <c r="E97" t="s">
         <v>2</v>
       </c>
-      <c r="D97">
+      <c r="F97">
         <v>6100</v>
       </c>
-      <c r="E97" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5">
+      <c r="G97" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98" s="1">
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C98" t="s">
+        <v>47</v>
+      </c>
+      <c r="D98" t="s">
+        <v>49</v>
+      </c>
+      <c r="E98" t="s">
         <v>4</v>
       </c>
-      <c r="D98">
+      <c r="F98">
         <v>2600</v>
       </c>
-      <c r="E98" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
+      <c r="G98" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99" s="1">
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C99" t="s">
+        <v>47</v>
+      </c>
+      <c r="D99" t="s">
+        <v>50</v>
+      </c>
+      <c r="E99" t="s">
         <v>4</v>
       </c>
-      <c r="D99">
+      <c r="F99">
         <v>1000</v>
       </c>
-      <c r="E99" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5">
+      <c r="G99" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C100" t="s">
+        <v>47</v>
+      </c>
+      <c r="D100" t="s">
+        <v>50</v>
+      </c>
+      <c r="E100" t="s">
         <v>4</v>
       </c>
-      <c r="D100">
+      <c r="F100">
         <v>1500</v>
       </c>
-      <c r="E100" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5">
+      <c r="G100" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101" s="1">
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C101" t="s">
+        <v>47</v>
+      </c>
+      <c r="D101" t="s">
+        <v>51</v>
+      </c>
+      <c r="E101" t="s">
         <v>2</v>
       </c>
-      <c r="D101">
+      <c r="F101">
         <v>1000</v>
       </c>
-      <c r="E101" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5">
+      <c r="G101" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7">
       <c r="A102" s="1">
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C102" t="s">
+        <v>47</v>
+      </c>
+      <c r="D102" t="s">
+        <v>49</v>
+      </c>
+      <c r="E102" t="s">
         <v>4</v>
       </c>
-      <c r="D102">
+      <c r="F102">
         <v>1000</v>
       </c>
-      <c r="E102" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="103" spans="1:5">
+      <c r="G102" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7">
       <c r="A103" s="1">
         <v>101</v>
       </c>
       <c r="B103" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C103" t="s">
+        <v>47</v>
+      </c>
+      <c r="D103" t="s">
+        <v>50</v>
+      </c>
+      <c r="E103" t="s">
         <v>5</v>
       </c>
-      <c r="D103">
+      <c r="F103">
         <v>500</v>
       </c>
-      <c r="E103" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5">
+      <c r="G103" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7">
       <c r="A104" s="1">
         <v>102</v>
       </c>
       <c r="B104" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C104" t="s">
+        <v>47</v>
+      </c>
+      <c r="D104" t="s">
+        <v>51</v>
+      </c>
+      <c r="E104" t="s">
         <v>7</v>
       </c>
-      <c r="D104">
+      <c r="F104">
         <v>500</v>
       </c>
-      <c r="E104" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5">
+      <c r="G104" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7">
       <c r="A105" s="1">
         <v>103</v>
       </c>
       <c r="B105" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C105" t="s">
+        <v>48</v>
+      </c>
+      <c r="D105" t="s">
+        <v>49</v>
+      </c>
+      <c r="E105" t="s">
         <v>8</v>
       </c>
-      <c r="D105">
+      <c r="F105">
         <v>500</v>
       </c>
-      <c r="E105" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="106" spans="1:5">
+      <c r="G105" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7">
       <c r="A106" s="1">
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C106" t="s">
+        <v>48</v>
+      </c>
+      <c r="D106" t="s">
+        <v>50</v>
+      </c>
+      <c r="E106" t="s">
         <v>2</v>
       </c>
-      <c r="D106">
+      <c r="F106">
         <v>1000</v>
       </c>
-      <c r="E106" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5">
+      <c r="G106" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7">
       <c r="A107" s="1">
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C107" t="s">
+        <v>48</v>
+      </c>
+      <c r="D107" t="s">
+        <v>51</v>
+      </c>
+      <c r="E107" t="s">
         <v>3</v>
       </c>
-      <c r="D107">
+      <c r="F107">
         <v>100</v>
       </c>
-      <c r="E107" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5">
+      <c r="G107" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7">
       <c r="A108" s="1">
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C108" t="s">
+        <v>48</v>
+      </c>
+      <c r="D108" t="s">
+        <v>49</v>
+      </c>
+      <c r="E108" t="s">
         <v>5</v>
       </c>
-      <c r="D108">
+      <c r="F108">
         <v>500</v>
       </c>
-      <c r="E108" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5">
+      <c r="G108" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7">
       <c r="A109" s="1">
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C109" t="s">
+        <v>48</v>
+      </c>
+      <c r="D109" t="s">
+        <v>50</v>
+      </c>
+      <c r="E109" t="s">
         <v>7</v>
       </c>
-      <c r="D109">
+      <c r="F109">
         <v>300</v>
       </c>
-      <c r="E109" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5">
+      <c r="G109" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7">
       <c r="A110" s="1">
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C110" t="s">
+        <v>48</v>
+      </c>
+      <c r="D110" t="s">
+        <v>50</v>
+      </c>
+      <c r="E110" t="s">
         <v>8</v>
       </c>
-      <c r="D110">
+      <c r="F110">
         <v>300</v>
       </c>
-      <c r="E110" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5">
+      <c r="G110" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7">
       <c r="A111" s="1">
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C111" t="s">
+        <v>48</v>
+      </c>
+      <c r="D111" t="s">
+        <v>51</v>
+      </c>
+      <c r="E111" t="s">
         <v>9</v>
       </c>
-      <c r="D111">
+      <c r="F111">
         <v>150</v>
       </c>
-      <c r="E111" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5">
+      <c r="G111" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7">
       <c r="A112" s="1">
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C112" t="s">
+        <v>48</v>
+      </c>
+      <c r="D112" t="s">
+        <v>50</v>
+      </c>
+      <c r="E112" t="s">
         <v>4</v>
       </c>
-      <c r="D112">
+      <c r="F112">
         <v>750</v>
       </c>
-      <c r="E112" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5">
+      <c r="G112" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7">
       <c r="A113" s="1">
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C113" t="s">
+        <v>48</v>
+      </c>
+      <c r="D113" t="s">
+        <v>50</v>
+      </c>
+      <c r="E113" t="s">
         <v>7</v>
       </c>
-      <c r="D113">
+      <c r="F113">
         <v>300</v>
       </c>
-      <c r="E113" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5">
+      <c r="G113" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7">
       <c r="A114" s="1">
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C114" t="s">
+        <v>48</v>
+      </c>
+      <c r="D114" t="s">
+        <v>49</v>
+      </c>
+      <c r="E114" t="s">
         <v>8</v>
       </c>
-      <c r="D114">
+      <c r="F114">
         <v>250</v>
       </c>
-      <c r="E114" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5">
+      <c r="G114" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7">
       <c r="A115" s="1">
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C115" t="s">
+        <v>48</v>
+      </c>
+      <c r="D115" t="s">
+        <v>50</v>
+      </c>
+      <c r="E115" t="s">
         <v>2</v>
       </c>
-      <c r="D115">
+      <c r="F115">
         <v>2500</v>
       </c>
-      <c r="E115" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5">
+      <c r="G115" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7">
       <c r="A116" s="1">
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C116" t="s">
+        <v>48</v>
+      </c>
+      <c r="D116" t="s">
+        <v>50</v>
+      </c>
+      <c r="E116" t="s">
         <v>4</v>
       </c>
-      <c r="D116">
+      <c r="F116">
         <v>1750</v>
       </c>
-      <c r="E116" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="117" spans="1:5">
+      <c r="G116" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7">
       <c r="A117" s="1">
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C117" t="s">
+        <v>48</v>
+      </c>
+      <c r="D117" t="s">
+        <v>51</v>
+      </c>
+      <c r="E117" t="s">
         <v>2</v>
       </c>
-      <c r="D117">
+      <c r="F117">
         <v>18700</v>
       </c>
-      <c r="E117" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="118" spans="1:5">
+      <c r="G117" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7">
       <c r="A118" s="1">
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C118" t="s">
+        <v>48</v>
+      </c>
+      <c r="D118" t="s">
+        <v>49</v>
+      </c>
+      <c r="E118" t="s">
         <v>4</v>
       </c>
-      <c r="D118">
+      <c r="F118">
         <v>6850</v>
       </c>
-      <c r="E118" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5">
+      <c r="G118" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7">
       <c r="A119" s="1">
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C119" t="s">
+        <v>48</v>
+      </c>
+      <c r="D119" t="s">
+        <v>50</v>
+      </c>
+      <c r="E119" t="s">
         <v>5</v>
       </c>
-      <c r="D119">
+      <c r="F119">
         <v>1500</v>
       </c>
-      <c r="E119" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5">
+      <c r="G119" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7">
       <c r="A120" s="1">
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C120" t="s">
+        <v>48</v>
+      </c>
+      <c r="D120" t="s">
+        <v>50</v>
+      </c>
+      <c r="E120" t="s">
         <v>6</v>
       </c>
-      <c r="D120">
+      <c r="F120">
         <v>1650</v>
       </c>
-      <c r="E120" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="121" spans="1:5">
+      <c r="G120" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7">
       <c r="A121" s="1">
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C121" t="s">
+        <v>48</v>
+      </c>
+      <c r="D121" t="s">
+        <v>51</v>
+      </c>
+      <c r="E121" t="s">
         <v>7</v>
       </c>
-      <c r="D121">
+      <c r="F121">
         <v>3000</v>
       </c>
-      <c r="E121" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5">
+      <c r="G121" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7">
       <c r="A122" s="1">
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C122" t="s">
+        <v>48</v>
+      </c>
+      <c r="D122" t="s">
+        <v>51</v>
+      </c>
+      <c r="E122" t="s">
         <v>8</v>
       </c>
-      <c r="D122">
+      <c r="F122">
         <v>2500</v>
       </c>
-      <c r="E122" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="123" spans="1:5">
+      <c r="G122" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7">
       <c r="A123" s="1">
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C123" t="s">
+        <v>48</v>
+      </c>
+      <c r="D123" t="s">
+        <v>49</v>
+      </c>
+      <c r="E123" t="s">
         <v>2</v>
       </c>
-      <c r="D123">
+      <c r="F123">
         <v>3000</v>
       </c>
-      <c r="E123" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5">
+      <c r="G123" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7">
       <c r="A124" s="1">
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C124" t="s">
+        <v>48</v>
+      </c>
+      <c r="D124" t="s">
+        <v>50</v>
+      </c>
+      <c r="E124" t="s">
         <v>2</v>
       </c>
-      <c r="D124">
+      <c r="F124">
         <v>600</v>
       </c>
-      <c r="E124" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5">
+      <c r="G124" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7">
       <c r="A125" s="1">
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C125" t="s">
+        <v>48</v>
+      </c>
+      <c r="D125" t="s">
+        <v>50</v>
+      </c>
+      <c r="E125" t="s">
         <v>2</v>
       </c>
-      <c r="D125">
+      <c r="F125">
         <v>1500</v>
       </c>
-      <c r="E125" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="126" spans="1:5">
+      <c r="G125" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7">
       <c r="A126" s="1">
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C126" t="s">
+        <v>48</v>
+      </c>
+      <c r="D126" t="s">
+        <v>51</v>
+      </c>
+      <c r="E126" t="s">
         <v>2</v>
       </c>
-      <c r="D126">
+      <c r="F126">
         <v>200</v>
       </c>
-      <c r="E126" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5">
+      <c r="G126" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7">
       <c r="A127" s="1">
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C127" t="s">
+        <v>48</v>
+      </c>
+      <c r="D127" t="s">
+        <v>50</v>
+      </c>
+      <c r="E127" t="s">
         <v>2</v>
       </c>
-      <c r="D127">
+      <c r="F127">
         <v>1500</v>
       </c>
-      <c r="E127" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5">
+      <c r="G127" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7">
       <c r="A128" s="1">
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C128" t="s">
+        <v>48</v>
+      </c>
+      <c r="D128" t="s">
+        <v>50</v>
+      </c>
+      <c r="E128" t="s">
         <v>2</v>
       </c>
-      <c r="D128">
+      <c r="F128">
         <v>2000</v>
       </c>
-      <c r="E128" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="129" spans="1:5">
+      <c r="G128" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7">
       <c r="A129" s="1">
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C129" t="s">
+        <v>48</v>
+      </c>
+      <c r="D129" t="s">
+        <v>49</v>
+      </c>
+      <c r="E129" t="s">
         <v>7</v>
       </c>
-      <c r="D129">
+      <c r="F129">
         <v>300</v>
       </c>
-      <c r="E129" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="130" spans="1:5">
+      <c r="G129" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7">
       <c r="A130" s="1">
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C130" t="s">
+        <v>48</v>
+      </c>
+      <c r="D130" t="s">
+        <v>50</v>
+      </c>
+      <c r="E130" t="s">
         <v>8</v>
       </c>
-      <c r="D130">
+      <c r="F130">
         <v>200</v>
       </c>
-      <c r="E130" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="131" spans="1:5">
+      <c r="G130" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7">
       <c r="A131" s="1">
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C131" t="s">
+        <v>48</v>
+      </c>
+      <c r="D131" t="s">
+        <v>50</v>
+      </c>
+      <c r="E131" t="s">
         <v>2</v>
       </c>
-      <c r="D131">
+      <c r="F131">
         <v>1800</v>
       </c>
-      <c r="E131" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5">
+      <c r="G131" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7">
       <c r="A132" s="1">
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C132" t="s">
+        <v>48</v>
+      </c>
+      <c r="D132" t="s">
+        <v>51</v>
+      </c>
+      <c r="E132" t="s">
         <v>7</v>
       </c>
-      <c r="D132">
+      <c r="F132">
         <v>200</v>
       </c>
-      <c r="E132" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5">
+      <c r="G132" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7">
       <c r="A133" s="1">
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C133" t="s">
+        <v>48</v>
+      </c>
+      <c r="D133" t="s">
+        <v>49</v>
+      </c>
+      <c r="E133" t="s">
         <v>8</v>
       </c>
-      <c r="D133">
+      <c r="F133">
         <v>200</v>
       </c>
-      <c r="E133" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="134" spans="1:5">
+      <c r="G133" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7">
       <c r="A134" s="1">
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C134" t="s">
+        <v>48</v>
+      </c>
+      <c r="D134" t="s">
+        <v>50</v>
+      </c>
+      <c r="E134" t="s">
         <v>2</v>
       </c>
-      <c r="D134">
+      <c r="F134">
         <v>1000</v>
       </c>
-      <c r="E134" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5">
+      <c r="G134" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7">
       <c r="A135" s="1">
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C135" t="s">
+        <v>48</v>
+      </c>
+      <c r="D135" t="s">
+        <v>50</v>
+      </c>
+      <c r="E135" t="s">
         <v>2</v>
       </c>
-      <c r="D135">
+      <c r="F135">
         <v>1000</v>
       </c>
-      <c r="E135" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5">
+      <c r="G135" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7">
       <c r="A136" s="1">
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C136" t="s">
+        <v>48</v>
+      </c>
+      <c r="D136" t="s">
+        <v>51</v>
+      </c>
+      <c r="E136" t="s">
         <v>7</v>
       </c>
-      <c r="D136">
+      <c r="F136">
         <v>500</v>
       </c>
-      <c r="E136" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5">
+      <c r="G136" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7">
       <c r="A137" s="1">
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C137" t="s">
+        <v>48</v>
+      </c>
+      <c r="D137" t="s">
+        <v>50</v>
+      </c>
+      <c r="E137" t="s">
         <v>8</v>
       </c>
-      <c r="D137">
+      <c r="F137">
         <v>500</v>
       </c>
-      <c r="E137" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5">
+      <c r="G137" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7">
       <c r="A138" s="1">
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C138" t="s">
+        <v>48</v>
+      </c>
+      <c r="D138" t="s">
+        <v>51</v>
+      </c>
+      <c r="E138" t="s">
         <v>2</v>
       </c>
-      <c r="D138">
+      <c r="F138">
         <v>650</v>
       </c>
-      <c r="E138" t="s">
-        <v>137</v>
+      <c r="G138" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>